<commit_message>
Inclusão de Ano nas tabelas
Inclusão de Ano nas tabelas
</commit_message>
<xml_diff>
--- a/DadosTratados/Distribuição da população, por cor ou raça, com indicação do coeficiente de variação, segundo Grandes Regiões e Unidades da Federação.xlsx
+++ b/DadosTratados/Distribuição da população, por cor ou raça, com indicação do coeficiente de variação, segundo Grandes Regiões e Unidades da Federação.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\ProjetoA3_BigData2021\DadosTratados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E02603C-78A5-48A9-B361-BC41FCB8AD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CB8EC5-01A0-44A5-8D28-97A054C2E9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="5" xr2:uid="{F5130B99-5930-4492-BB99-C1E1528D2553}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{F5130B99-5930-4492-BB99-C1E1528D2553}"/>
   </bookViews>
   <sheets>
     <sheet name="2012" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="40">
   <si>
     <t>-</t>
   </si>
@@ -156,6 +156,9 @@
   <si>
     <t>Preta Total</t>
   </si>
+  <si>
+    <t>Ano:</t>
+  </si>
 </sst>
 </file>
 
@@ -189,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -225,11 +228,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -246,6 +258,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E62254-49C2-4429-8A22-1742D0847EE7}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,9 +591,10 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -608,8 +628,11 @@
       <c r="K1" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -643,8 +666,11 @@
       <c r="K2" s="2">
         <v>22.655376294190617</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -678,8 +704,11 @@
       <c r="K3" s="2">
         <v>34.005835059069454</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -713,8 +742,11 @@
       <c r="K4" s="2">
         <v>26.985788614768907</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -748,8 +780,11 @@
       <c r="K5" s="2">
         <v>27.026556544880297</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -783,8 +818,11 @@
       <c r="K6" s="2">
         <v>17.973978895018245</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -818,8 +856,11 @@
       <c r="K7" s="2">
         <v>93.55577309532481</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -853,8 +894,11 @@
       <c r="K8" s="2">
         <v>20.883331757182905</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -888,8 +932,11 @@
       <c r="K9" s="2">
         <v>14.138552673348121</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -923,8 +970,11 @@
       <c r="K10" s="2">
         <v>78.255606232848294</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -958,8 +1008,11 @@
       <c r="K11" s="2">
         <v>15.991517528379534</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -993,8 +1046,11 @@
       <c r="K12" s="2">
         <v>39.739037669239799</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1028,8 +1084,11 @@
       <c r="K13" s="2">
         <v>91.134723397475398</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1063,8 +1122,11 @@
       <c r="K14" s="2">
         <v>20.340404754881742</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1098,8 +1160,11 @@
       <c r="K15" s="2">
         <v>25.858234487582859</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1133,8 +1198,11 @@
       <c r="K16" s="2">
         <v>26.931340252267518</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1168,8 +1236,11 @@
       <c r="K17" s="2">
         <v>15.69181432055089</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1203,8 +1274,11 @@
       <c r="K18" s="2">
         <v>15.579589190710214</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -1238,8 +1312,11 @@
       <c r="K19" s="2">
         <v>18.490309756512584</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1273,8 +1350,11 @@
       <c r="K20" s="2">
         <v>16.769489586880777</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1308,8 +1388,11 @@
       <c r="K21" s="2">
         <v>9.9941884215201426</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1343,8 +1426,11 @@
       <c r="K22" s="2">
         <v>11.613590021480315</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1378,8 +1464,11 @@
       <c r="K23" s="2">
         <v>20.181459116078628</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -1413,8 +1502,11 @@
       <c r="K24" s="2">
         <v>18.562397152330636</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -1448,8 +1540,11 @@
       <c r="K25" s="2">
         <v>17.815140681871892</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1483,8 +1578,11 @@
       <c r="K26" s="2">
         <v>18.983266641151726</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1518,8 +1616,11 @@
       <c r="K27" s="2">
         <v>29.950710370304851</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -1552,6 +1653,9 @@
       </c>
       <c r="K28" s="2">
         <v>21.047466763049059</v>
+      </c>
+      <c r="L28" s="7">
+        <v>2012</v>
       </c>
     </row>
   </sheetData>
@@ -1561,15 +1665,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A912BE6-02C5-4472-B5A9-62B1618308B9}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L6" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="9.140625" style="8"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1603,8 +1710,11 @@
       <c r="K1" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1638,8 +1748,11 @@
       <c r="K2" s="2">
         <v>21.457563294052999</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1673,8 +1786,11 @@
       <c r="K3" s="2">
         <v>30.856201874276739</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1708,8 +1824,11 @@
       <c r="K4" s="2">
         <v>28.129372447031521</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1743,8 +1862,11 @@
       <c r="K5" s="2">
         <v>21.275388694530719</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1778,8 +1900,11 @@
       <c r="K6" s="2">
         <v>20.329825564879421</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1813,8 +1938,11 @@
       <c r="K7" s="2">
         <v>42.5010904370099</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1848,8 +1976,11 @@
       <c r="K8" s="2">
         <v>24.681601869306931</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1883,8 +2014,11 @@
       <c r="K9" s="2">
         <v>22.408017019944246</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1918,8 +2052,11 @@
       <c r="K10" s="2">
         <v>53.887491133822522</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1953,8 +2090,11 @@
       <c r="K11" s="2">
         <v>19.039509468814899</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1988,8 +2128,11 @@
       <c r="K12" s="2">
         <v>30.999003968846207</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -2023,8 +2166,11 @@
       <c r="K13" s="2">
         <v>23.267386500207092</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -2058,8 +2204,11 @@
       <c r="K14" s="2">
         <v>21.527451817732633</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -2093,8 +2242,11 @@
       <c r="K15" s="2">
         <v>21.436442876448446</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -2128,8 +2280,11 @@
       <c r="K16" s="2">
         <v>20.188278328361619</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -2163,8 +2318,11 @@
       <c r="K17" s="2">
         <v>16.351361623941074</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -2198,8 +2356,11 @@
       <c r="K18" s="2">
         <v>17.956387494518232</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -2233,8 +2394,11 @@
       <c r="K19" s="2">
         <v>18.310246000407819</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -2268,8 +2432,11 @@
       <c r="K20" s="2">
         <v>19.000682893908248</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -2303,8 +2470,11 @@
       <c r="K21" s="2">
         <v>10.392226238191721</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -2338,8 +2508,11 @@
       <c r="K22" s="2">
         <v>14.489108356849117</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -2373,8 +2546,11 @@
       <c r="K23" s="2">
         <v>22.827869794458636</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -2408,8 +2584,11 @@
       <c r="K24" s="2">
         <v>21.493778326813086</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -2443,8 +2622,11 @@
       <c r="K25" s="2">
         <v>16.781485408330301</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -2478,8 +2660,11 @@
       <c r="K26" s="2">
         <v>18.862107527485708</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -2513,8 +2698,11 @@
       <c r="K27" s="2">
         <v>27.502554275555909</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -2547,6 +2735,9 @@
       </c>
       <c r="K28" s="2">
         <v>18.360655855653889</v>
+      </c>
+      <c r="L28" s="7">
+        <v>2013</v>
       </c>
     </row>
   </sheetData>
@@ -2556,15 +2747,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BEB9BD-612B-4D71-8E7B-CAF7F9E652AD}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L4" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="9.140625" style="8"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2598,8 +2792,11 @@
       <c r="K1" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2633,8 +2830,11 @@
       <c r="K2" s="2">
         <v>26.073481236735603</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2668,8 +2868,11 @@
       <c r="K3" s="2">
         <v>36.762752065760225</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2703,8 +2906,11 @@
       <c r="K4" s="2">
         <v>39.277922404161956</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2738,8 +2944,11 @@
       <c r="K5" s="2">
         <v>18.646344171524653</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -2773,8 +2982,11 @@
       <c r="K6" s="2">
         <v>19.7308262997052</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2808,8 +3020,11 @@
       <c r="K7" s="2">
         <v>32.695693697810427</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -2843,8 +3058,11 @@
       <c r="K8" s="2">
         <v>36.004997705377683</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2878,8 +3096,11 @@
       <c r="K9" s="2">
         <v>18.70158541315655</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -2913,8 +3134,11 @@
       <c r="K10" s="2">
         <v>76.184715947994775</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -2948,8 +3172,11 @@
       <c r="K11" s="2">
         <v>30.307039933068609</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -2983,8 +3210,11 @@
       <c r="K12" s="2">
         <v>29.105820231605982</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -3018,8 +3248,11 @@
       <c r="K13" s="2">
         <v>40.095542067211923</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -3053,8 +3286,11 @@
       <c r="K14" s="2">
         <v>38.591183885783529</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -3088,8 +3324,11 @@
       <c r="K15" s="2">
         <v>38.11779319368263</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -3123,8 +3362,11 @@
       <c r="K16" s="2">
         <v>20.080418086271067</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -3158,8 +3400,11 @@
       <c r="K17" s="2">
         <v>19.280795190257852</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -3193,8 +3438,11 @@
       <c r="K18" s="2">
         <v>24.372205844376939</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -3228,8 +3476,11 @@
       <c r="K19" s="2">
         <v>22.888662976425607</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -3263,8 +3514,11 @@
       <c r="K20" s="2">
         <v>18.694596856119009</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -3298,8 +3552,11 @@
       <c r="K21" s="2">
         <v>12.261289072083947</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -3333,8 +3590,11 @@
       <c r="K22" s="2">
         <v>12.481466718182032</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -3368,8 +3628,11 @@
       <c r="K23" s="2">
         <v>21.450907975896865</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -3403,8 +3666,11 @@
       <c r="K24" s="2">
         <v>19.73308927179275</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -3438,8 +3704,11 @@
       <c r="K25" s="2">
         <v>17.089532589115212</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -3473,8 +3742,11 @@
       <c r="K26" s="2">
         <v>20.792652590658793</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -3508,8 +3780,11 @@
       <c r="K27" s="2">
         <v>36.366151222772153</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -3542,6 +3817,9 @@
       </c>
       <c r="K28" s="2">
         <v>21.863191914118385</v>
+      </c>
+      <c r="L28" s="7">
+        <v>2014</v>
       </c>
     </row>
   </sheetData>
@@ -3551,15 +3829,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FA50B3-7301-4CC9-9630-3A9B92C09C81}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L4" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="9.140625" style="8"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -3593,8 +3874,11 @@
       <c r="K1" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3628,8 +3912,11 @@
       <c r="K2" s="2">
         <v>34.062003356221787</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -3663,8 +3950,11 @@
       <c r="K3" s="2">
         <v>31.337050427971864</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -3698,8 +3988,11 @@
       <c r="K4" s="2">
         <v>29.219505750724906</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -3733,8 +4026,11 @@
       <c r="K5" s="2">
         <v>25.376948834453245</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -3768,8 +4064,11 @@
       <c r="K6" s="2">
         <v>23.229333793064193</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -3803,8 +4102,11 @@
       <c r="K7" s="2">
         <v>64.404698050136005</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -3838,8 +4140,11 @@
       <c r="K8" s="2">
         <v>26.713323876949769</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -3873,8 +4178,11 @@
       <c r="K9" s="2">
         <v>20.278697081301029</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -3908,8 +4216,11 @@
       <c r="K10" s="2">
         <v>49.331028810699344</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -3943,8 +4254,11 @@
       <c r="K11" s="2">
         <v>19.575280762537577</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -3978,8 +4292,11 @@
       <c r="K12" s="2">
         <v>46.703004549669807</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -4013,8 +4330,11 @@
       <c r="K13" s="2">
         <v>31.243239091243403</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -4048,8 +4368,11 @@
       <c r="K14" s="2">
         <v>18.883985345508485</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -4083,8 +4406,11 @@
       <c r="K15" s="2">
         <v>37.446714421900573</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -4118,8 +4444,11 @@
       <c r="K16" s="2">
         <v>27.852335302123421</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -4153,8 +4482,11 @@
       <c r="K17" s="2">
         <v>18.035045640668191</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -4188,8 +4520,11 @@
       <c r="K18" s="2">
         <v>19.938306958689989</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -4223,8 +4558,11 @@
       <c r="K19" s="2">
         <v>18.434267141494136</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -4258,8 +4596,11 @@
       <c r="K20" s="2">
         <v>19.195802977175916</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -4293,8 +4634,11 @@
       <c r="K21" s="2">
         <v>9.6759512351930237</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -4328,8 +4672,11 @@
       <c r="K22" s="2">
         <v>12.790536299392283</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -4363,8 +4710,11 @@
       <c r="K23" s="2">
         <v>21.079091218084319</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -4398,8 +4748,11 @@
       <c r="K24" s="2">
         <v>17.869902499330255</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -4433,8 +4786,11 @@
       <c r="K25" s="2">
         <v>20.434005468687687</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -4468,8 +4824,11 @@
       <c r="K26" s="2">
         <v>20.438763603689921</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -4503,8 +4862,11 @@
       <c r="K27" s="2">
         <v>22.307206194184712</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -4537,6 +4899,9 @@
       </c>
       <c r="K28" s="2">
         <v>19.065374215874012</v>
+      </c>
+      <c r="L28" s="7">
+        <v>2015</v>
       </c>
     </row>
   </sheetData>
@@ -4546,15 +4911,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD5D82F-455C-4351-A40E-3884337D71C9}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L4" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="9.140625" style="8"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -4588,8 +4956,11 @@
       <c r="K1" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -4623,8 +4994,11 @@
       <c r="K2" s="2">
         <v>19.059960033756678</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -4658,8 +5032,11 @@
       <c r="K3" s="2">
         <v>32.5190877531995</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -4693,8 +5070,11 @@
       <c r="K4" s="2">
         <v>21.413009513048653</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -4728,8 +5108,11 @@
       <c r="K5" s="2">
         <v>22.595181107013786</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -4763,8 +5146,11 @@
       <c r="K6" s="2">
         <v>15.971347030490717</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4798,8 +5184,11 @@
       <c r="K7" s="2">
         <v>52.506331629551198</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -4833,8 +5222,11 @@
       <c r="K8" s="2">
         <v>23.198410080349635</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -4868,8 +5260,11 @@
       <c r="K9" s="2">
         <v>13.496790913106288</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -4903,8 +5298,11 @@
       <c r="K10" s="2">
         <v>36.228108576037606</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -4938,8 +5336,11 @@
       <c r="K11" s="2">
         <v>18.204707337112179</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -4973,8 +5374,11 @@
       <c r="K12" s="2">
         <v>26.039762967685874</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -5008,8 +5412,11 @@
       <c r="K13" s="2">
         <v>29.480350311027543</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -5043,8 +5450,11 @@
       <c r="K14" s="2">
         <v>15.078525005591709</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -5078,8 +5488,11 @@
       <c r="K15" s="2">
         <v>22.037271880262413</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -5113,8 +5526,11 @@
       <c r="K16" s="2">
         <v>18.050679850892394</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -5148,8 +5564,11 @@
       <c r="K17" s="2">
         <v>17.754340739692427</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -5183,8 +5602,11 @@
       <c r="K18" s="2">
         <v>18.010392867793001</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -5218,8 +5640,11 @@
       <c r="K19" s="2">
         <v>15.725934923896906</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -5253,8 +5678,11 @@
       <c r="K20" s="2">
         <v>13.152880966046865</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -5288,8 +5716,11 @@
       <c r="K21" s="2">
         <v>9.1617940928232233</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -5323,8 +5754,11 @@
       <c r="K22" s="2">
         <v>14.884638402885972</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -5358,8 +5792,11 @@
       <c r="K23" s="2">
         <v>20.009378676999077</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -5393,8 +5830,11 @@
       <c r="K24" s="2">
         <v>19.882882626820209</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -5428,8 +5868,11 @@
       <c r="K25" s="2">
         <v>15.621013390690546</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -5463,8 +5906,11 @@
       <c r="K26" s="2">
         <v>17.818904387887688</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -5498,8 +5944,11 @@
       <c r="K27" s="2">
         <v>16.099466271156167</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -5532,6 +5981,9 @@
       </c>
       <c r="K28" s="2">
         <v>19.530972220311952</v>
+      </c>
+      <c r="L28" s="7">
+        <v>2016</v>
       </c>
     </row>
   </sheetData>
@@ -5541,15 +5993,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71BD49DE-733D-4C2F-845D-8E33F735E048}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="9.140625" style="8"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -5583,8 +6038,11 @@
       <c r="K1" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -5618,8 +6076,11 @@
       <c r="K2" s="2">
         <v>18.143454346628332</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -5653,8 +6114,11 @@
       <c r="K3" s="2">
         <v>29.431522986088083</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5688,8 +6152,11 @@
       <c r="K4" s="2">
         <v>23.280669714019027</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -5723,8 +6190,11 @@
       <c r="K5" s="2">
         <v>20.612814547544168</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -5758,8 +6228,11 @@
       <c r="K6" s="2">
         <v>19.699031500211632</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -5793,8 +6266,11 @@
       <c r="K7" s="2">
         <v>50.128857329572071</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -5828,8 +6304,11 @@
       <c r="K8" s="2">
         <v>20.258438390612454</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -5863,8 +6342,11 @@
       <c r="K9" s="2">
         <v>11.029842925410275</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -5898,8 +6380,11 @@
       <c r="K10" s="2">
         <v>41.118290322099114</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -5933,8 +6418,11 @@
       <c r="K11" s="2">
         <v>20.047207685649845</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -5968,8 +6456,11 @@
       <c r="K12" s="2">
         <v>33.001431948084189</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -6003,8 +6494,11 @@
       <c r="K13" s="2">
         <v>30.948377954501321</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -6038,8 +6532,11 @@
       <c r="K14" s="2">
         <v>15.199993297788739</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -6073,8 +6570,11 @@
       <c r="K15" s="2">
         <v>16.192959549211054</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -6108,8 +6608,11 @@
       <c r="K16" s="2">
         <v>20.458747418314267</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -6143,8 +6646,11 @@
       <c r="K17" s="2">
         <v>16.107265444130149</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -6178,8 +6684,11 @@
       <c r="K18" s="2">
         <v>17.865326372292319</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -6213,8 +6722,11 @@
       <c r="K19" s="2">
         <v>17.77879595968481</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -6248,8 +6760,11 @@
       <c r="K20" s="2">
         <v>12.934282921630627</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -6283,8 +6798,11 @@
       <c r="K21" s="2">
         <v>8.7214175742665301</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -6318,8 +6836,11 @@
       <c r="K22" s="2">
         <v>11.647222037095869</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -6353,8 +6874,11 @@
       <c r="K23" s="2">
         <v>17.708248194516603</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -6388,8 +6912,11 @@
       <c r="K24" s="2">
         <v>17.7081660718348</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -6423,8 +6950,11 @@
       <c r="K25" s="2">
         <v>15.119215132369144</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -6458,8 +6988,11 @@
       <c r="K26" s="2">
         <v>15.876647693338922</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -6493,8 +7026,11 @@
       <c r="K27" s="2">
         <v>18.558256119447165</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -6527,6 +7063,9 @@
       </c>
       <c r="K28" s="2">
         <v>38.08064610852724</v>
+      </c>
+      <c r="L28" s="7">
+        <v>2017</v>
       </c>
     </row>
   </sheetData>
@@ -6536,10 +7075,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26E1342-B4CE-467F-8FB0-0364D246517B}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:K1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6549,9 +7088,10 @@
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -6585,8 +7125,11 @@
       <c r="K1" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -6620,8 +7163,11 @@
       <c r="K2" s="2">
         <v>16.849394120737571</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -6655,8 +7201,11 @@
       <c r="K3" s="2">
         <v>16.701582156157571</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -6690,8 +7239,11 @@
       <c r="K4" s="2">
         <v>19.096522530759042</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -6725,8 +7277,11 @@
       <c r="K5" s="2">
         <v>14.383915479843232</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -6760,8 +7315,11 @@
       <c r="K6" s="2">
         <v>12.734195995226619</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -6795,8 +7353,11 @@
       <c r="K7" s="2">
         <v>22.590979854278174</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -6830,8 +7391,11 @@
       <c r="K8" s="2">
         <v>16.481885194126278</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -6865,8 +7429,11 @@
       <c r="K9" s="2">
         <v>7.9139495492813374</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -6900,8 +7467,11 @@
       <c r="K10" s="2">
         <v>27.211818380344781</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -6935,8 +7505,11 @@
       <c r="K11" s="2">
         <v>13.869715900756056</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -6970,8 +7543,11 @@
       <c r="K12" s="2">
         <v>34.404307291540768</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -7005,8 +7581,11 @@
       <c r="K13" s="2">
         <v>18.763584987625432</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -7040,8 +7619,11 @@
       <c r="K14" s="2">
         <v>12.708970294527166</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -7075,8 +7657,11 @@
       <c r="K15" s="2">
         <v>14.879801742635864</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -7110,8 +7695,11 @@
       <c r="K16" s="2">
         <v>15.409708434307037</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -7145,8 +7733,11 @@
       <c r="K17" s="2">
         <v>12.292297709509601</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -7180,8 +7771,11 @@
       <c r="K18" s="2">
         <v>15.148539190312702</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -7215,8 +7809,11 @@
       <c r="K19" s="2">
         <v>10.579811730196084</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -7250,8 +7847,11 @@
       <c r="K20" s="2">
         <v>10.238355191050797</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -7285,8 +7885,11 @@
       <c r="K21" s="2">
         <v>9.6038544708210374</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -7320,8 +7923,11 @@
       <c r="K22" s="2">
         <v>9.9591179591667878</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -7355,8 +7961,11 @@
       <c r="K23" s="2">
         <v>15.193663260991585</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -7390,8 +7999,11 @@
       <c r="K24" s="2">
         <v>16.982863310209662</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -7425,8 +8037,11 @@
       <c r="K25" s="2">
         <v>14.458758049863929</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -7460,8 +8075,11 @@
       <c r="K26" s="2">
         <v>30.013639623102133</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -7495,8 +8113,11 @@
       <c r="K27" s="2">
         <v>14.380795767025392</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -7529,6 +8150,9 @@
       </c>
       <c r="K28" s="2">
         <v>24.858496438286085</v>
+      </c>
+      <c r="L28" s="7">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>